<commit_message>
add: freshly generated reports
</commit_message>
<xml_diff>
--- a/src/test/resources/Output.xlsx
+++ b/src/test/resources/Output.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="94">
   <si>
     <t>Doctor Name</t>
   </si>
@@ -294,6 +294,15 @@
   </si>
   <si>
     <t>Adyar,Chennai  Dent Eazee Speciality Dental Centres</t>
+  </si>
+  <si>
+    <t>Dr. Abhilash Bhaskaran</t>
+  </si>
+  <si>
+    <t>Perumbakkam,Chennai  Gleneagles Health City + 1 more</t>
+  </si>
+  <si>
+    <t>₹800 Consultation fee at clinic</t>
   </si>
 </sst>
 </file>
@@ -649,19 +658,19 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>87</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s" s="0">
         <v>6</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>88</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
@@ -717,19 +726,19 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>17</v>
+        <v>91</v>
       </c>
       <c r="B6" t="s" s="0">
         <v>6</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>19</v>
+        <v>92</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>13</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>